<commit_message>
Establish the preliminary framework for the project (with AI assistance)
</commit_message>
<xml_diff>
--- a/data/province_info.xlsx
+++ b/data/province_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15124\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Interactive-Culture-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D596A2A-D34A-4AEA-925E-E7A955080C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD3EA10-3817-4AE6-A227-515B671D05A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{EEDC0187-CA75-4BF5-A515-8F38C88CBF36}"/>
   </bookViews>
@@ -389,469 +389,469 @@
     <t>甘肃省</t>
   </si>
   <si>
+    <t>宁夏回族自治区</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新疆维吾尔自治区</t>
+  </si>
+  <si>
+    <t>zainayaoyuandedifang.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在那遥远的地方</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zai Na Yao Yuan De Di Fang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qinghai</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>In that Distant Land</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天津市</t>
+  </si>
+  <si>
+    <t>上海市</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆市</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉林省</t>
+  </si>
+  <si>
+    <t>辽宁省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>贵州省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖南省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖北省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>海南省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回娘家</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>huiniangjia.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hui Niang Jia</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Returning to Mother's Home</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>山歌好比春江水</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小拜年</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shangehaobichunjiangshui.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guangxi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shan Ge Hao Bi Chun Jiang Shui</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Folk songs are like the spring river water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xiao Bai Nian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Paying A New Year Call </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiaobainian.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liaoning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanlushibawan.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>山路十八弯</t>
+  </si>
+  <si>
+    <t>Shan Lu Shi Ba Wan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hubei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xizang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qing Zang Gao Yuan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qinghai-Tibet Plateau</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>青藏高原</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qingzanggaoyuan.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hunan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>浏阳河</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Yang He</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Yang River</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>liuyanghe.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>采茶舞曲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cai Cha Wu Qu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caichawuqu.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fengyanghuagu.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>凤阳花鼓</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anhui</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feng Yang Hua Gu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fengyang Drum Dance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jilin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>满堂红</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Man Tang Hong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mantanghong.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qingnichangdaohainanlai.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hainan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>请你常到海南来</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please Visit Hainan Often</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qing Ni Chang Dao Hai Nan Lai</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zuimeiguizhou.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guizhou</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>醉美贵州</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drunkenly Beautiful Guizhou</t>
+  </si>
+  <si>
+    <t>Zui Mei Gui Zhou</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tea-Picking Dance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Welcome to Beijing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Girls of Alishan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Azalea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eighteen Winding Mountain Roads</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All-round Success</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizizhige_aomen.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aomen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>七子之歌：澳门</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qi Zi Zhi Ge: Ao Men</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Song of the Seven Sons: Macau</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>helanshan.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ningxia</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>贺兰山</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>He Lan Shan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xinjiang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tianjin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanghai</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chongqing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qingchunwuqu.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>青春舞曲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qing Chun Wu Qu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Youth Dance Tune</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tianjinwawa.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tian Jin Wa Wa</t>
+  </si>
+  <si>
+    <t>Tianjin Kids</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天津娃娃</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>妹妹的山丹花儿开</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meimeideshandanhuaerkai.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mei Mei De Shan Dan Hua Er Kai</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beauty's Rhododendron Blossoms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guangdong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>海阔天空</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>haikuotiankong.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hai Kuo Tian Kong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boundless Oceans, Vast Skies</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fujian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gansu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>taiyangchulaixiyangyang.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>太阳出来喜洋洋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Sun Rises, Joy Abounds </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tian Yang Chu Lai Xi Yang Yang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caichage.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>采茶歌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cai Cha Ge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tea-Picking Song</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yelaixiang.mp3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>夜来香</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ye Lai Xiang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Night-blooming jasmine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helan Mountains</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>澳门特别行政区</t>
-  </si>
-  <si>
-    <t>宁夏回族自治区</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>新疆维吾尔自治区</t>
-  </si>
-  <si>
-    <t>zainayaoyuandedifang.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>在那遥远的地方</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zai Na Yao Yuan De Di Fang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qinghai</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>In that Distant Land</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>天津市</t>
-  </si>
-  <si>
-    <t>上海市</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>重庆市</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>吉林省</t>
-  </si>
-  <si>
-    <t>辽宁省</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>贵州省</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>湖南省</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>湖北省</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>海南省</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>回娘家</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>huiniangjia.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hui Niang Jia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Returning to Mother's Home</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>山歌好比春江水</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>小拜年</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shangehaobichunjiangshui.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Guangxi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shan Ge Hao Bi Chun Jiang Shui</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Folk songs are like the spring river water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Xiao Bai Nian</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Paying A New Year Call </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>xiaobainian.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liaoning</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shanlushibawan.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>山路十八弯</t>
-  </si>
-  <si>
-    <t>Shan Lu Shi Ba Wan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hubei</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Xizang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qing Zang Gao Yuan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qinghai-Tibet Plateau</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>青藏高原</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>qingzanggaoyuan.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hunan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>浏阳河</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Yang He</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Yang River</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>liuyanghe.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>采茶舞曲</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cai Cha Wu Qu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caichawuqu.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fengyanghuagu.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>凤阳花鼓</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Anhui</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Feng Yang Hua Gu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fengyang Drum Dance</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jilin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>满堂红</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Man Tang Hong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mantanghong.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>qingnichangdaohainanlai.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hainan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>请你常到海南来</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Please Visit Hainan Often</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qing Ni Chang Dao Hai Nan Lai</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zuimeiguizhou.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Guizhou</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>醉美贵州</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Drunkenly Beautiful Guizhou</t>
-  </si>
-  <si>
-    <t>Zui Mei Gui Zhou</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tea-Picking Dance</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Welcome to Beijing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Girls of Alishan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Azalea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eighteen Winding Mountain Roads</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>All-round Success</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>qizizhige_aomen.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aomen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>七子之歌：澳门</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qi Zi Zhi Ge: Ao Men</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Song of the Seven Sons: Macau</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>helanshan.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ningxia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>贺兰山</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>He Lan Shan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helan Mountains
-Helan Mountains</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Xinjiang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tianjin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shanghai</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chongqing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>qingchunwuqu.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>青春舞曲</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qing Chun Wu Qu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Youth Dance Tune</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tianjinwawa.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tian Jin Wa Wa</t>
-  </si>
-  <si>
-    <t>Tianjin Kids</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>天津娃娃</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>妹妹的山丹花儿开</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>meimeideshandanhuaerkai.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mei Mei De Shan Dan Hua Er Kai</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Beauty's Rhododendron Blossoms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Guangdong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>海阔天空</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>haikuotiankong.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hai Kuo Tian Kong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boundless Oceans, Vast Skies</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fujian</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gansu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>taiyangchulaixiyangyang.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>太阳出来喜洋洋</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Sun Rises, Joy Abounds </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tian Yang Chu Lai Xi Yang Yang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caichage.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>采茶歌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cai Cha Ge</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tea-Picking Song</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yelaixiang.mp3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>夜来香</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ye Lai Xiang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Night-blooming jasmine</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1408,16 +1408,16 @@
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
         <v>109</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -1468,16 +1468,16 @@
         <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -1494,7 +1494,7 @@
         <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F11" t="s">
         <v>44</v>
@@ -1554,7 +1554,7 @@
         <v>63</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F14" t="s">
         <v>65</v>
@@ -1574,7 +1574,7 @@
         <v>69</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F15" t="s">
         <v>76</v>
@@ -1605,19 +1605,19 @@
         <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -1625,19 +1625,19 @@
         <v>86</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="F18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -1645,19 +1645,19 @@
         <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -1665,19 +1665,19 @@
         <v>88</v>
       </c>
       <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -1685,19 +1685,19 @@
         <v>89</v>
       </c>
       <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" t="s">
         <v>130</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
@@ -1705,19 +1705,19 @@
         <v>90</v>
       </c>
       <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C22" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="F22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -1725,259 +1725,259 @@
         <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" t="s">
-        <v>167</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="B25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" t="s">
         <v>169</v>
-      </c>
-      <c r="F24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" t="s">
-        <v>171</v>
-      </c>
-      <c r="C25" t="s">
-        <v>172</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="F26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="F28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" t="s">
         <v>120</v>
-      </c>
-      <c r="F30" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s">
         <v>145</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" t="s">
         <v>147</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F31" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" t="s">
         <v>155</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" t="s">
         <v>156</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E32" t="s">
-        <v>157</v>
-      </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" t="s">
         <v>132</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" t="s">
         <v>135</v>
-      </c>
-      <c r="F33" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" t="s">
         <v>150</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="F35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>